<commit_message>
Finished analyssi for preliminary doubling time dilutions
</commit_message>
<xml_diff>
--- a/exp5_doublingtime_dilutions/exp5_plate.xlsx
+++ b/exp5_doublingtime_dilutions/exp5_plate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmdb/Ludington_rotation/exp5_doublingtime_dilutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C277A69-DA82-284B-A1A5-DB70E60687C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831DF8D8-F7BD-B647-81AB-34E720E8BF8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{788BCF0A-6E91-F640-BD07-40ED4B3CDE64}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -37,18 +37,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>1x Media</t>
@@ -422,7 +410,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,40 +459,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -512,40 +500,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -553,40 +541,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -594,46 +582,44 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -648,43 +634,19 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="A7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="A8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>

</xml_diff>